<commit_message>
fix : RR-HR-RAS001 bom fix
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/RR-HL-RAS001.xlsx
+++ b/機械設計/_BOM/RR-HL-RAS001.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9358C576-90B5-4BA3-AC13-516920DFA27A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2A06F45-F3B1-48B7-8971-421BC6B21CD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17970" yWindow="13980" windowWidth="14400" windowHeight="10845" xr2:uid="{B0579A99-BF4D-4D8C-B463-97F4069799DE}"/>
+    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{A49F1F11-9A6F-44E3-AD9B-F424E636C652}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{4C1CD8FD-3576-47AE-99F9-5EC91F101D1E}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="932" windowWidth="960" windowHeight="723" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{8C0DA47F-24FE-4DFE-B0DB-F671AE91DD8C}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -137,7 +137,7 @@
     <t>RR-HL-RAS-P001</t>
   </si>
   <si>
-    <t>前足底</t>
+    <t>前足底右半身側</t>
   </si>
   <si>
     <t>購入品</t>
@@ -266,8 +266,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{2BEE7B13-1556-41E1-8A67-E178DEC6C12E}">
-  <header guid="{2BEE7B13-1556-41E1-8A67-E178DEC6C12E}" dateTime="2023-07-12T19:35:17" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{F9E485F8-749C-4557-91D9-9FBF3A9DBCE0}">
+  <header guid="{F9E485F8-749C-4557-91D9-9FBF3A9DBCE0}" dateTime="2023-07-13T14:36:17" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -579,7 +579,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A77CF1-5412-4C9C-AE2E-B63A23EDDAF9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09B89213-6BFB-4F15-98BC-C01BD9EF8E15}">
   <dimension ref="A1:S9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -591,7 +591,7 @@
     <col min="3" max="3" width="16.125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="5.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="6.5" bestFit="1" customWidth="1"/>
@@ -985,7 +985,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{4C1CD8FD-3576-47AE-99F9-5EC91F101D1E}">
+    <customSheetView guid="{8C0DA47F-24FE-4DFE-B0DB-F671AE91DD8C}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>